<commit_message>
javascript, index.html überarbeitet, datenbank file hinzugefügt, stunden aktualisiert
</commit_message>
<xml_diff>
--- a/administratives/2020S_CE KT_Zeitaufzeichnung_Gruppe9.xlsx
+++ b/administratives/2020S_CE KT_Zeitaufzeichnung_Gruppe9.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stefa\Dropbox\Uni\Uni\SS 2020\CE KT\VS Anwendung\CEKT-Web\administratives\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stefan_SRV01\Desktop\URL Shortener\GIT Repository\CEKT-Web\administratives\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E4937AA-C5B0-4A15-84B2-BF978E05C8EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0F3B99A-E2C0-475B-B46F-6C1428ED74FD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,9 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext uri="GoogleSheetsCustomDataVersion1">
@@ -36,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="32">
   <si>
     <t>Name:</t>
   </si>
@@ -129,6 +127,9 @@
   </si>
   <si>
     <t>SQLite Datenbank auf dem Server aufsetzen, erste Table erstellen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Erste HTML Page erstellt, Javascript Anwendung eingelesen und ausprobiert </t>
   </si>
 </sst>
 </file>
@@ -273,7 +274,7 @@
         <name val="Calibri"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="165" formatCode="hh:mm"/>
+      <numFmt numFmtId="25" formatCode="hh:mm"/>
     </dxf>
     <dxf>
       <font>
@@ -291,7 +292,7 @@
         <name val="Calibri"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="165" formatCode="hh:mm"/>
+      <numFmt numFmtId="25" formatCode="hh:mm"/>
     </dxf>
     <dxf>
       <font>
@@ -322,7 +323,7 @@
         <name val="Calibri"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="165" formatCode="hh:mm"/>
+      <numFmt numFmtId="25" formatCode="hh:mm"/>
     </dxf>
     <dxf>
       <font>
@@ -340,7 +341,7 @@
         <name val="Calibri"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="165" formatCode="hh:mm"/>
+      <numFmt numFmtId="25" formatCode="hh:mm"/>
     </dxf>
     <dxf>
       <font>
@@ -371,7 +372,7 @@
         <name val="Calibri"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="165" formatCode="hh:mm"/>
+      <numFmt numFmtId="25" formatCode="hh:mm"/>
     </dxf>
     <dxf>
       <font>
@@ -389,7 +390,7 @@
         <name val="Calibri"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="165" formatCode="hh:mm"/>
+      <numFmt numFmtId="25" formatCode="hh:mm"/>
     </dxf>
     <dxf>
       <fill>
@@ -882,11 +883,11 @@
       </c>
       <c r="D6" s="7">
         <f>SUMIF('Hinterhölzl Stefan'!$E$5:$E$31,Übersicht!$A6,'Hinterhölzl Stefan'!$G$5:$G$31)</f>
-        <v>1.0000000000000018</v>
+        <v>2.5000000000000004</v>
       </c>
       <c r="E6" s="7">
         <f>SUM(Übersicht!$B6:$D6)</f>
-        <v>1.0000000000000018</v>
+        <v>2.5000000000000004</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -966,11 +967,11 @@
       </c>
       <c r="D10" s="12">
         <f t="shared" si="0"/>
-        <v>9.0000000000000018</v>
+        <v>10.5</v>
       </c>
       <c r="E10" s="12">
         <f>SUM(Übersicht!$B10:$D10)</f>
-        <v>26</v>
+        <v>27.5</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5573,7 +5574,7 @@
   <dimension ref="A1:W996"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5600,7 +5601,7 @@
       </c>
       <c r="E1" s="5">
         <f>SUM('Hinterhölzl Stefan'!$G$5:$G$27)</f>
-        <v>9.0000000000000018</v>
+        <v>10.5</v>
       </c>
     </row>
     <row r="2" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -5775,18 +5776,28 @@
       <c r="W7" s="8"/>
     </row>
     <row r="8" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="9"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
+      <c r="A8" s="9">
+        <v>43916</v>
+      </c>
+      <c r="B8" s="10">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="C8" s="10">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>14</v>
+      </c>
       <c r="F8" s="10">
         <f>'Hinterhölzl Stefan'!$C8-'Hinterhölzl Stefan'!$B8</f>
-        <v>0</v>
+        <v>6.2499999999999944E-2</v>
       </c>
       <c r="G8" s="19">
         <f>'Hinterhölzl Stefan'!$F8*24</f>
-        <v>0</v>
+        <v>1.4999999999999987</v>
       </c>
       <c r="Q8" s="6"/>
       <c r="R8" s="13"/>

</xml_diff>

<commit_message>
Zeit eingetagen zu voheriger Arbeit
</commit_message>
<xml_diff>
--- a/administratives/2020S_CE KT_Zeitaufzeichnung_Gruppe9.xlsx
+++ b/administratives/2020S_CE KT_Zeitaufzeichnung_Gruppe9.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stefan_SRV01\Desktop\URL Shortener\GIT Repository\CEKT-Web\administratives\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0F3B99A-E2C0-475B-B46F-6C1428ED74FD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{102BC362-0BC0-49C4-BCE4-503CA5113152}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3015" yWindow="3510" windowWidth="21600" windowHeight="11385" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Übersicht" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="33">
   <si>
     <t>Name:</t>
   </si>
@@ -130,6 +130,9 @@
   </si>
   <si>
     <t xml:space="preserve">Erste HTML Page erstellt, Javascript Anwendung eingelesen und ausprobiert </t>
+  </si>
+  <si>
+    <t>Verbindung SQLite - Visual Code, erste Tests mit node.js</t>
   </si>
 </sst>
 </file>
@@ -883,11 +886,11 @@
       </c>
       <c r="D6" s="7">
         <f>SUMIF('Hinterhölzl Stefan'!$E$5:$E$31,Übersicht!$A6,'Hinterhölzl Stefan'!$G$5:$G$31)</f>
-        <v>2.5000000000000004</v>
+        <v>6.0000000000000018</v>
       </c>
       <c r="E6" s="7">
         <f>SUM(Übersicht!$B6:$D6)</f>
-        <v>2.5000000000000004</v>
+        <v>6.0000000000000018</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -967,11 +970,11 @@
       </c>
       <c r="D10" s="12">
         <f t="shared" si="0"/>
-        <v>10.5</v>
+        <v>14.000000000000002</v>
       </c>
       <c r="E10" s="12">
         <f>SUM(Übersicht!$B10:$D10)</f>
-        <v>27.5</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5574,7 +5577,7 @@
   <dimension ref="A1:W996"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5601,7 +5604,7 @@
       </c>
       <c r="E1" s="5">
         <f>SUM('Hinterhölzl Stefan'!$G$5:$G$27)</f>
-        <v>10.5</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -5808,18 +5811,28 @@
       <c r="W8" s="6"/>
     </row>
     <row r="9" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="9"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
+      <c r="A9" s="9">
+        <v>43916</v>
+      </c>
+      <c r="B9" s="10">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C9" s="10">
+        <v>0.8125</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>14</v>
+      </c>
       <c r="F9" s="10">
         <f>'Hinterhölzl Stefan'!$C9-'Hinterhölzl Stefan'!$B9</f>
-        <v>0</v>
+        <v>0.14583333333333337</v>
       </c>
       <c r="G9" s="19">
         <f>'Hinterhölzl Stefan'!$F9*24</f>
-        <v>0</v>
+        <v>3.5000000000000009</v>
       </c>
       <c r="H9" s="14"/>
       <c r="I9" s="8"/>

</xml_diff>

<commit_message>
Testapp.js läuft, script.js noch nicht
</commit_message>
<xml_diff>
--- a/administratives/2020S_CE KT_Zeitaufzeichnung_Gruppe9.xlsx
+++ b/administratives/2020S_CE KT_Zeitaufzeichnung_Gruppe9.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stefan_SRV01\Desktop\URL Shortener\GIT Repository\CEKT-Web\administratives\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{102BC362-0BC0-49C4-BCE4-503CA5113152}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5F2722A-FF70-495F-BCBC-58F42568532F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3015" yWindow="3510" windowWidth="21600" windowHeight="11385" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="34">
   <si>
     <t>Name:</t>
   </si>
@@ -133,6 +133,9 @@
   </si>
   <si>
     <t>Verbindung SQLite - Visual Code, erste Tests mit node.js</t>
+  </si>
+  <si>
+    <t>Javascript SQL Querry über HTML Button starten - Versuche</t>
   </si>
 </sst>
 </file>
@@ -886,11 +889,11 @@
       </c>
       <c r="D6" s="7">
         <f>SUMIF('Hinterhölzl Stefan'!$E$5:$E$31,Übersicht!$A6,'Hinterhölzl Stefan'!$G$5:$G$31)</f>
-        <v>6.0000000000000018</v>
+        <v>6.7500000000000018</v>
       </c>
       <c r="E6" s="7">
         <f>SUM(Übersicht!$B6:$D6)</f>
-        <v>6.0000000000000018</v>
+        <v>6.7500000000000018</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -970,11 +973,11 @@
       </c>
       <c r="D10" s="12">
         <f t="shared" si="0"/>
-        <v>14.000000000000002</v>
+        <v>14.750000000000002</v>
       </c>
       <c r="E10" s="12">
         <f>SUM(Übersicht!$B10:$D10)</f>
-        <v>31</v>
+        <v>31.75</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5577,7 +5580,7 @@
   <dimension ref="A1:W996"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5604,7 +5607,7 @@
       </c>
       <c r="E1" s="5">
         <f>SUM('Hinterhölzl Stefan'!$G$5:$G$27)</f>
-        <v>14</v>
+        <v>14.75</v>
       </c>
     </row>
     <row r="2" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -5852,18 +5855,28 @@
       <c r="W9" s="8"/>
     </row>
     <row r="10" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="9"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
+      <c r="A10" s="9">
+        <v>43916</v>
+      </c>
+      <c r="B10" s="10">
+        <v>0.89583333333333337</v>
+      </c>
+      <c r="C10" s="10">
+        <v>0.92708333333333337</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>14</v>
+      </c>
       <c r="F10" s="10">
         <f>'Hinterhölzl Stefan'!$C10-'Hinterhölzl Stefan'!$B10</f>
-        <v>0</v>
+        <v>3.125E-2</v>
       </c>
       <c r="G10" s="19">
         <f>'Hinterhölzl Stefan'!$F10*24</f>
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="H10" s="8"/>
       <c r="I10" s="8"/>

</xml_diff>

<commit_message>
warum muss i jeds moi commiten?
</commit_message>
<xml_diff>
--- a/administratives/2020S_CE KT_Zeitaufzeichnung_Gruppe9.xlsx
+++ b/administratives/2020S_CE KT_Zeitaufzeichnung_Gruppe9.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomas\Dropbox\AAA OwnShare\JKU-Linz\4. Sem\CE KT Web\CEKT-Web\administratives\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AB9A789-28A6-4336-ABB3-90963DD72AEA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4D6BAE0-90A4-49B9-B5C8-606E4567A37F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="36">
   <si>
     <t>Name:</t>
   </si>
@@ -139,6 +139,9 @@
   </si>
   <si>
     <t>überarbeitung Lernvertrag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Erreichbarkeit Server </t>
   </si>
 </sst>
 </file>
@@ -884,7 +887,7 @@
       </c>
       <c r="B6" s="7">
         <f>SUMIF('Deutsch Thomas'!$E$5:$E$27,Übersicht!$A6,'Deutsch Thomas'!$G$5:$G$27)</f>
-        <v>0</v>
+        <v>2.0000000000000009</v>
       </c>
       <c r="C6" s="7">
         <f>SUMIF('Bolda Stefan'!$E$5:$E$27,Übersicht!$A6,'Bolda Stefan'!$G$5:$G$27)</f>
@@ -896,7 +899,7 @@
       </c>
       <c r="E6" s="7">
         <f>SUM(Übersicht!$B6:$D6)</f>
-        <v>6.7500000000000018</v>
+        <v>8.7500000000000036</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -968,7 +971,7 @@
       </c>
       <c r="B10" s="12">
         <f t="shared" ref="B10:D10" si="0">SUM(B4:B9)</f>
-        <v>9.5000000000000036</v>
+        <v>11.500000000000004</v>
       </c>
       <c r="C10" s="12">
         <f t="shared" si="0"/>
@@ -980,7 +983,7 @@
       </c>
       <c r="E10" s="12">
         <f>SUM(Übersicht!$B10:$D10)</f>
-        <v>32.250000000000007</v>
+        <v>34.250000000000007</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1987,7 +1990,7 @@
   <dimension ref="A1:W996"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2014,7 +2017,7 @@
       </c>
       <c r="E1" s="5">
         <f>SUM('Deutsch Thomas'!$G$5:$G$27)</f>
-        <v>9.5</v>
+        <v>11.5</v>
       </c>
     </row>
     <row r="2" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2221,18 +2224,28 @@
       <c r="W8" s="3"/>
     </row>
     <row r="9" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="9"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
+      <c r="A9" s="9">
+        <v>43924</v>
+      </c>
+      <c r="B9" s="10">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C9" s="10">
+        <v>0.75</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>14</v>
+      </c>
       <c r="F9" s="10">
         <f>'Deutsch Thomas'!$C9-'Deutsch Thomas'!$B9</f>
-        <v>0</v>
+        <v>8.333333333333337E-2</v>
       </c>
       <c r="G9" s="19">
         <f>'Deutsch Thomas'!$F9*24</f>
-        <v>0</v>
+        <v>2.0000000000000009</v>
       </c>
       <c r="H9" s="14"/>
       <c r="I9" s="8"/>

</xml_diff>

<commit_message>
Frontend - Post Delete Get
</commit_message>
<xml_diff>
--- a/administratives/2020S_CE KT_Zeitaufzeichnung_Gruppe9.xlsx
+++ b/administratives/2020S_CE KT_Zeitaufzeichnung_Gruppe9.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stefa\Dropbox\Uni\Uni\SS 2020\CE KT\VS Anwendung\CEKT-Web\administratives\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14505289-E47D-4246-A86F-88EEC402C7C8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{682D349F-FDFE-4AFC-ABD7-9B041DABB76A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="43">
   <si>
     <t>Name:</t>
   </si>
@@ -160,6 +160,9 @@
   </si>
   <si>
     <t>Frontend weiterentwickeln, erste Restcalls von der Webpage</t>
+  </si>
+  <si>
+    <t>Frontend weiterentwickelt, Get, Post, Delete möglich - aber kein Errorhandling</t>
   </si>
 </sst>
 </file>
@@ -913,11 +916,11 @@
       </c>
       <c r="D6" s="7">
         <f>SUMIF('Hinterhölzl Stefan'!$E$5:$E$31,Übersicht!$A6,'Hinterhölzl Stefan'!$G$5:$G$31)</f>
-        <v>18.250000000000004</v>
+        <v>21.250000000000004</v>
       </c>
       <c r="E6" s="7">
         <f>SUM(Übersicht!$B6:$D6)</f>
-        <v>33.000000000000007</v>
+        <v>36.000000000000007</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -997,11 +1000,11 @@
       </c>
       <c r="D10" s="12">
         <f t="shared" si="0"/>
-        <v>26.250000000000004</v>
+        <v>29.250000000000004</v>
       </c>
       <c r="E10" s="12">
         <f>SUM(Übersicht!$B10:$D10)</f>
-        <v>58.500000000000014</v>
+        <v>61.500000000000014</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5664,7 +5667,7 @@
   <dimension ref="A1:W996"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5691,7 +5694,7 @@
       </c>
       <c r="E1" s="5">
         <f>SUM('Hinterhölzl Stefan'!$G$5:$G$27)</f>
-        <v>26.25</v>
+        <v>29.25</v>
       </c>
     </row>
     <row r="2" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6144,18 +6147,28 @@
       <c r="W14" s="8"/>
     </row>
     <row r="15" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="9"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
+      <c r="A15" s="9">
+        <v>43927</v>
+      </c>
+      <c r="B15" s="10">
+        <v>0.875</v>
+      </c>
+      <c r="C15" s="10">
+        <v>1</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>14</v>
+      </c>
       <c r="F15" s="10">
         <f>'Hinterhölzl Stefan'!$C15-'Hinterhölzl Stefan'!$B15</f>
-        <v>0</v>
+        <v>0.125</v>
       </c>
       <c r="G15" s="19">
         <f>'Hinterhölzl Stefan'!$F15*24</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H15" s="14"/>
       <c r="I15" s="14"/>

</xml_diff>